<commit_message>
[bug] fixed some game data issues
</commit_message>
<xml_diff>
--- a/data/games/Game_1_17-09-2022.xlsx
+++ b/data/games/Game_1_17-09-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanuel.woldekidan/gitrepos/flamingo_stats/data/games/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55BED43-C79F-C744-AC83-343F020BEB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41176BA-3688-2B4E-8465-CF0AAE7D97B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="3" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="27040" activeTab="1" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
   <si>
     <t>Flamingo Fadaways</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>Tehrani R.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -642,10 +639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084FA9C7-071B-744B-9071-1A20F95C2B9B}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,11 +841,6 @@
         <v>29</v>
       </c>
       <c r="H9" s="2"/>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I26" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1054,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A9B0DD-A295-D744-9B94-C8207D40001D}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>

</xml_diff>